<commit_message>
update with 3 pts example
</commit_message>
<xml_diff>
--- a/affine_2d_office_script/affine_2d_transformation.xlsx
+++ b/affine_2d_office_script/affine_2d_transformation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Farid\gitProjects\coordinate_transformations\affine_2d_office_script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wsponlinenam-my.sharepoint.com/personal/farid_javadnejad_wsp_com/Documents/Documents/GitHub/coordinate_transformations/affine_2d_office_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD00EFBA-3F5A-4C69-BF11-98ABB883FAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{FD00EFBA-3F5A-4C69-BF11-98ABB883FAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F958226-31FB-4EB9-B776-19FDDF7CFE0F}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{CE33CA41-0F61-4C0E-ACEE-51F901476334}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>PID</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Residuals</t>
+  </si>
+  <si>
+    <t>=</t>
   </si>
 </sst>
 </file>
@@ -127,12 +130,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,166 +597,185 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C77EB3-7BC0-4E98-B2DD-6D40A82168F8}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A2" sqref="A2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2">
         <v>1840.6385519466176</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2">
         <v>0.99999291672147783</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2">
         <v>-3.7714982338895864E-3</v>
       </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2">
         <v>-2509.0282761909184</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2">
         <v>3.7713401845838601E-3</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2">
         <v>0.99999256559775562</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11" s="2">
+      <c r="C11" s="2">
         <v>0</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>1.1641532182693479E-10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
-      <c r="B12" s="2">
+      <c r="C12" s="2">
         <v>1.1641532182693479E-10</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D12" s="2">
         <v>-2.9103830456733704E-10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
-      <c r="B13" s="2">
+      <c r="C13" s="2">
         <v>-1.1641532182693479E-10</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>1.7462298274040222E-10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="2">
+      <c r="C15" s="2">
         <v>1.1641532182693479E-10</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D15" s="2">
         <v>2.9103830456733704E-10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="2">
+      <c r="C16" s="2">
         <v>7.7610214551289872E-11</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D16" s="2">
         <v>1.9402553637822467E-10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="2">
+      <c r="C17" s="2">
         <v>9.5052712239293153E-11</v>
       </c>
-      <c r="C17" s="2">
+      <c r="D17" s="2">
         <v>2.0716258348026526E-10</v>
       </c>
     </row>
@@ -762,11 +785,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<scriptIds xmlns="http://schemas.microsoft.com/office/extensibility/maker/v1.0" id="script-ids-node-id">
-  <scriptId id="ms-officescript%3A%2F%2Fonedrive_business_itemlink%2F01TEUQH5JGYQCQPUNTB5AJZ3NEFDAWWD2O:ms-officescript%3A%2F%2Fonedrive_business_sharinglink%2Fu!aHR0cHM6Ly93c3BvbmxpbmVuYW0tbXkuc2hhcmVwb2ludC5jb20vOnU6L2cvcGVyc29uYWwvZmFyaWRfamF2YWRuZWphZF93c3BfY29tL0VTYkVCUWZSc3c5QW5PMmtLTUZyRDA0QmpDaVB3NHFRc2VHYjcySGdkSHlVWHc"/>
-  <scriptId xmlns="" id="ms-officescript%3A%2F%2Fsharepoint_itemlink%2Fb!0U0Cf1YnG0CvWwc6jpbAWWxeiTfW8-5FqP9Co3hJpTg7s_RU5d1WSqx8IF0brNt8%2F016EEM6J6AXZAXLAAGOFGJBMP5QJXJQPII:ms-officescript%3A%2F%2Fsharepoint_sharinglink%2Fu!aHR0cHM6Ly93c3BvbmxpbmVuYW0uc2hhcmVwb2ludC5jb20vOnU6L3MvVVMtU291dGh3ZXN0LUdlb21hdGkvRWNDLVFYV0FCbkZNa0xIOWdtNllQUWdCZUMzSnFFaTVVVTljSWF1cmxaRjFOQQ"/>
-  <scriptId xmlns="" id="ms-officescript%3A%2F%2Fsharepoint_itemlink%2Fb!0U0Cf1YnG0CvWwc6jpbAWWxeiTfW8-5FqP9Co3hJpTg7s_RU5d1WSqx8IF0brNt8%2F016EEM6J2Z7CGCQDCKKJDKGNSR3WYRJ4AU:ms-officescript%3A%2F%2Fsharepoint_sharinglink%2Fu!aHR0cHM6Ly93c3BvbmxpbmVuYW0uc2hhcmVwb2ludC5jb20vOnU6L3MvVVMtU291dGh3ZXN0LUdlb21hdGkvRVZuNGpDZ01TbEpHb3paUjNiRVU4QlFCVDRMVFRrMHBPQ1JWWVRCcFdQaUxsZw"/>
-</scriptIds>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -781,12 +805,11 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<scriptIds xmlns="http://schemas.microsoft.com/office/extensibility/maker/v1.0" id="script-ids-node-id">
+  <scriptId id="ms-officescript%3A%2F%2Fonedrive_business_itemlink%2F01TEUQH5JGYQCQPUNTB5AJZ3NEFDAWWD2O:ms-officescript%3A%2F%2Fonedrive_business_sharinglink%2Fu!aHR0cHM6Ly93c3BvbmxpbmVuYW0tbXkuc2hhcmVwb2ludC5jb20vOnU6L2cvcGVyc29uYWwvZmFyaWRfamF2YWRuZWphZF93c3BfY29tL0VTYkVCUWZSc3c5QW5PMmtLTUZyRDA0QmpDaVB3NHFRc2VHYjcySGdkSHlVWHc"/>
+  <scriptId xmlns="" id="ms-officescript%3A%2F%2Fsharepoint_itemlink%2Fb!0U0Cf1YnG0CvWwc6jpbAWWxeiTfW8-5FqP9Co3hJpTg7s_RU5d1WSqx8IF0brNt8%2F016EEM6J6AXZAXLAAGOFGJBMP5QJXJQPII:ms-officescript%3A%2F%2Fsharepoint_sharinglink%2Fu!aHR0cHM6Ly93c3BvbmxpbmVuYW0uc2hhcmVwb2ludC5jb20vOnU6L3MvVVMtU291dGh3ZXN0LUdlb21hdGkvRWNDLVFYV0FCbkZNa0xIOWdtNllQUWdCZUMzSnFFaTVVVTljSWF1cmxaRjFOQQ"/>
+  <scriptId xmlns="" id="ms-officescript%3A%2F%2Fsharepoint_itemlink%2Fb!0U0Cf1YnG0CvWwc6jpbAWWxeiTfW8-5FqP9Co3hJpTg7s_RU5d1WSqx8IF0brNt8%2F016EEM6J2Z7CGCQDCKKJDKGNSR3WYRJ4AU:ms-officescript%3A%2F%2Fsharepoint_sharinglink%2Fu!aHR0cHM6Ly93c3BvbmxpbmVuYW0uc2hhcmVwb2ludC5jb20vOnU6L3MvVVMtU291dGh3ZXN0LUdlb21hdGkvRVZuNGpDZ01TbEpHb3paUjNiRVU4QlFCVDRMVFRrMHBPQ1JWWVRCcFdQaUxsZw"/>
+</scriptIds>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1003,10 +1026,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1352322F-05A0-41DC-BE90-8969A90EF1CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F4439F3-FB71-4DD0-8297-953047485624}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/extensibility/maker/v1.0"/>
-    <ds:schemaRef ds:uri=""/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1023,9 +1045,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F4439F3-FB71-4DD0-8297-953047485624}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1352322F-05A0-41DC-BE90-8969A90EF1CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/extensibility/maker/v1.0"/>
+    <ds:schemaRef ds:uri=""/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>